<commit_message>
Bug fixes on regression problems. Score is not a percentage anymore. Plots are showed when regression problem is 1 feature, 1 target.
</commit_message>
<xml_diff>
--- a/examples/regression/Auto_Insurance_In_Sweden/data.xlsx
+++ b/examples/regression/Auto_Insurance_In_Sweden/data.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fofanama1\machine-learning\uipath_challenge\_Examples\Auto_Insurance_In_Sweden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fofanama1\machine-learning\uipath_challenge\HandyML\examples\regression\Auto_Insurance_In_Sweden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4FFBCA-4D00-4C2B-8BC0-79A6DFD79909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9FDBFE-B98F-4899-93EB-6262AD69B4C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="11430" xr2:uid="{3E10406B-08CA-4275-86A3-05E85B9174DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>